<commit_message>
Fix: harmonized chart colors and stacking order across Food–Land and Energy tabs; removed redundant transport column cleanup; cleaned data_loader warnings; updated interactive Energy chart layout; updated all data files with new interactive versions
</commit_message>
<xml_diff>
--- a/data/LEAP_Demand_Emissions.xlsx
+++ b/data/LEAP_Demand_Emissions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giann\Downloads\Telegram Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ev\Documents\Software Projects\SDSN GCH\ScenViz_Template\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97FF13C-591F-488B-AD57-8FCB7B6018DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1106CD-89A7-4A0F-85DB-5371DCB3AA6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{01BF1780-3214-47DB-9C17-C2F5550468A3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{01BF1780-3214-47DB-9C17-C2F5550468A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -116,9 +116,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;&quot;\-&quot;&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="170" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * &quot;&quot;\-&quot;&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -168,15 +168,15 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -514,23 +514,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23F58F65-D173-4C9B-B57C-646E19A136BF}">
   <dimension ref="A1:J320"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.1796875" customWidth="1"/>
-    <col min="8" max="8" width="13.1796875" customWidth="1"/>
-    <col min="9" max="9" width="12.54296875" customWidth="1"/>
-    <col min="10" max="10" width="22.81640625" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -562,7 +564,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>2022</v>
       </c>
@@ -594,7 +596,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2023</v>
       </c>
@@ -626,7 +628,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2024</v>
       </c>
@@ -658,7 +660,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2025</v>
       </c>
@@ -690,7 +692,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>2026</v>
       </c>
@@ -722,7 +724,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2027</v>
       </c>
@@ -754,7 +756,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2028</v>
       </c>
@@ -786,7 +788,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>2029</v>
       </c>
@@ -818,7 +820,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2030</v>
       </c>
@@ -850,7 +852,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2031</v>
       </c>
@@ -882,7 +884,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2032</v>
       </c>
@@ -914,7 +916,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>2033</v>
       </c>
@@ -946,7 +948,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2034</v>
       </c>
@@ -978,7 +980,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>2035</v>
       </c>
@@ -1010,7 +1012,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>2036</v>
       </c>
@@ -1042,7 +1044,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>2037</v>
       </c>
@@ -1074,7 +1076,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>2038</v>
       </c>
@@ -1106,7 +1108,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2039</v>
       </c>
@@ -1138,7 +1140,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>2040</v>
       </c>
@@ -1170,7 +1172,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>2041</v>
       </c>
@@ -1202,7 +1204,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>2042</v>
       </c>
@@ -1234,7 +1236,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>2043</v>
       </c>
@@ -1266,7 +1268,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>2044</v>
       </c>
@@ -1298,7 +1300,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>2045</v>
       </c>
@@ -1330,7 +1332,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>2046</v>
       </c>
@@ -1362,7 +1364,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>2047</v>
       </c>
@@ -1394,7 +1396,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>2048</v>
       </c>
@@ -1426,7 +1428,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>2049</v>
       </c>
@@ -1458,7 +1460,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>2050</v>
       </c>
@@ -1490,7 +1492,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>2022</v>
       </c>
@@ -1522,7 +1524,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>2023</v>
       </c>
@@ -1554,7 +1556,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>2024</v>
       </c>
@@ -1586,7 +1588,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>2025</v>
       </c>
@@ -1618,7 +1620,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>2026</v>
       </c>
@@ -1650,7 +1652,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>2027</v>
       </c>
@@ -1682,7 +1684,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>2028</v>
       </c>
@@ -1714,7 +1716,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>2029</v>
       </c>
@@ -1746,7 +1748,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>2030</v>
       </c>
@@ -1778,7 +1780,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>2031</v>
       </c>
@@ -1810,7 +1812,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>2032</v>
       </c>
@@ -1842,7 +1844,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>2033</v>
       </c>
@@ -1874,7 +1876,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>2034</v>
       </c>
@@ -1906,7 +1908,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>2035</v>
       </c>
@@ -1938,7 +1940,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>2036</v>
       </c>
@@ -1970,7 +1972,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>2037</v>
       </c>
@@ -2002,7 +2004,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>2038</v>
       </c>
@@ -2034,7 +2036,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>2039</v>
       </c>
@@ -2066,7 +2068,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>2040</v>
       </c>
@@ -2098,7 +2100,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>2041</v>
       </c>
@@ -2130,7 +2132,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>2042</v>
       </c>
@@ -2162,7 +2164,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>2043</v>
       </c>
@@ -2194,7 +2196,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>2044</v>
       </c>
@@ -2226,7 +2228,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>2045</v>
       </c>
@@ -2258,7 +2260,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>2046</v>
       </c>
@@ -2290,7 +2292,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>2047</v>
       </c>
@@ -2322,7 +2324,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>2048</v>
       </c>
@@ -2354,7 +2356,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>2049</v>
       </c>
@@ -2386,7 +2388,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>2050</v>
       </c>
@@ -2418,7 +2420,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>2022</v>
       </c>
@@ -2450,7 +2452,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>2023</v>
       </c>
@@ -2482,7 +2484,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>2024</v>
       </c>
@@ -2514,7 +2516,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>2025</v>
       </c>
@@ -2546,7 +2548,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>2026</v>
       </c>
@@ -2578,7 +2580,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>2027</v>
       </c>
@@ -2610,7 +2612,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>2028</v>
       </c>
@@ -2642,7 +2644,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>2029</v>
       </c>
@@ -2674,7 +2676,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>2030</v>
       </c>
@@ -2706,7 +2708,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>2031</v>
       </c>
@@ -2738,7 +2740,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>2032</v>
       </c>
@@ -2770,7 +2772,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>2033</v>
       </c>
@@ -2802,7 +2804,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>2034</v>
       </c>
@@ -2834,7 +2836,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>2035</v>
       </c>
@@ -2866,7 +2868,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>2036</v>
       </c>
@@ -2898,7 +2900,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>2037</v>
       </c>
@@ -2930,7 +2932,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>2038</v>
       </c>
@@ -2962,7 +2964,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>2039</v>
       </c>
@@ -2994,7 +2996,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>2040</v>
       </c>
@@ -3026,7 +3028,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>2041</v>
       </c>
@@ -3058,7 +3060,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>2042</v>
       </c>
@@ -3090,7 +3092,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>2043</v>
       </c>
@@ -3122,7 +3124,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>2044</v>
       </c>
@@ -3154,7 +3156,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>2045</v>
       </c>
@@ -3186,7 +3188,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>2046</v>
       </c>
@@ -3218,7 +3220,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>2047</v>
       </c>
@@ -3250,7 +3252,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>2048</v>
       </c>
@@ -3282,7 +3284,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>2049</v>
       </c>
@@ -3314,7 +3316,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>2050</v>
       </c>
@@ -3346,7 +3348,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>2022</v>
       </c>
@@ -3378,7 +3380,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>2023</v>
       </c>
@@ -3410,7 +3412,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>2024</v>
       </c>
@@ -3442,7 +3444,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>2025</v>
       </c>
@@ -3474,7 +3476,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>2026</v>
       </c>
@@ -3506,7 +3508,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>2027</v>
       </c>
@@ -3538,7 +3540,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>2028</v>
       </c>
@@ -3570,7 +3572,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>2029</v>
       </c>
@@ -3602,7 +3604,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>2030</v>
       </c>
@@ -3634,7 +3636,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>2031</v>
       </c>
@@ -3666,7 +3668,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>2032</v>
       </c>
@@ -3698,7 +3700,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>2033</v>
       </c>
@@ -3730,7 +3732,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>2034</v>
       </c>
@@ -3762,7 +3764,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>2035</v>
       </c>
@@ -3794,7 +3796,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>2036</v>
       </c>
@@ -3826,7 +3828,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>2037</v>
       </c>
@@ -3858,7 +3860,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>2038</v>
       </c>
@@ -3890,7 +3892,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>2039</v>
       </c>
@@ -3922,7 +3924,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>2040</v>
       </c>
@@ -3954,7 +3956,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>2041</v>
       </c>
@@ -3986,7 +3988,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>2042</v>
       </c>
@@ -4018,7 +4020,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>2043</v>
       </c>
@@ -4050,7 +4052,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>2044</v>
       </c>
@@ -4082,7 +4084,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>2045</v>
       </c>
@@ -4114,7 +4116,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>2046</v>
       </c>
@@ -4146,7 +4148,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>2047</v>
       </c>
@@ -4178,7 +4180,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>2048</v>
       </c>
@@ -4210,7 +4212,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>2049</v>
       </c>
@@ -4242,7 +4244,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>2050</v>
       </c>
@@ -4274,7 +4276,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>2022</v>
       </c>
@@ -4306,7 +4308,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>2023</v>
       </c>
@@ -4338,7 +4340,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>2024</v>
       </c>
@@ -4370,7 +4372,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>2025</v>
       </c>
@@ -4402,7 +4404,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>2026</v>
       </c>
@@ -4434,7 +4436,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>2027</v>
       </c>
@@ -4466,7 +4468,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>2028</v>
       </c>
@@ -4498,7 +4500,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>2029</v>
       </c>
@@ -4530,7 +4532,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>2030</v>
       </c>
@@ -4562,7 +4564,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>2031</v>
       </c>
@@ -4594,7 +4596,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>2032</v>
       </c>
@@ -4626,7 +4628,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>2033</v>
       </c>
@@ -4658,7 +4660,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>2034</v>
       </c>
@@ -4690,7 +4692,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>2035</v>
       </c>
@@ -4722,7 +4724,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>2036</v>
       </c>
@@ -4754,7 +4756,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>2037</v>
       </c>
@@ -4786,7 +4788,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>2038</v>
       </c>
@@ -4818,7 +4820,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>2039</v>
       </c>
@@ -4850,7 +4852,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>2040</v>
       </c>
@@ -4882,7 +4884,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>2041</v>
       </c>
@@ -4914,7 +4916,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>2042</v>
       </c>
@@ -4946,7 +4948,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>2043</v>
       </c>
@@ -4978,7 +4980,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>2044</v>
       </c>
@@ -5010,7 +5012,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>2045</v>
       </c>
@@ -5042,7 +5044,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>2046</v>
       </c>
@@ -5074,7 +5076,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>2047</v>
       </c>
@@ -5106,7 +5108,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>2048</v>
       </c>
@@ -5138,7 +5140,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>2049</v>
       </c>
@@ -5170,7 +5172,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>2050</v>
       </c>
@@ -5202,7 +5204,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>2022</v>
       </c>
@@ -5234,7 +5236,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>2023</v>
       </c>
@@ -5266,7 +5268,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>2024</v>
       </c>
@@ -5298,7 +5300,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>2025</v>
       </c>
@@ -5330,7 +5332,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>2026</v>
       </c>
@@ -5362,7 +5364,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>2027</v>
       </c>
@@ -5394,7 +5396,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>2028</v>
       </c>
@@ -5426,7 +5428,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>2029</v>
       </c>
@@ -5458,7 +5460,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>2030</v>
       </c>
@@ -5490,7 +5492,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>2031</v>
       </c>
@@ -5522,7 +5524,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>2032</v>
       </c>
@@ -5554,7 +5556,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>2033</v>
       </c>
@@ -5586,7 +5588,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>2034</v>
       </c>
@@ -5618,7 +5620,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>2035</v>
       </c>
@@ -5650,7 +5652,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>2036</v>
       </c>
@@ -5682,7 +5684,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>2037</v>
       </c>
@@ -5714,7 +5716,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>2038</v>
       </c>
@@ -5746,7 +5748,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>2039</v>
       </c>
@@ -5778,7 +5780,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>2040</v>
       </c>
@@ -5810,7 +5812,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>2041</v>
       </c>
@@ -5842,7 +5844,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="167" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>2042</v>
       </c>
@@ -5874,7 +5876,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="168" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>2043</v>
       </c>
@@ -5906,7 +5908,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>2044</v>
       </c>
@@ -5938,7 +5940,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>2045</v>
       </c>
@@ -5970,7 +5972,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="171" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>2046</v>
       </c>
@@ -6002,7 +6004,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>2047</v>
       </c>
@@ -6034,7 +6036,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>2048</v>
       </c>
@@ -6066,7 +6068,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="174" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>2049</v>
       </c>
@@ -6098,7 +6100,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>2050</v>
       </c>
@@ -6130,7 +6132,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="176" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>2022</v>
       </c>
@@ -6162,7 +6164,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>2023</v>
       </c>
@@ -6194,7 +6196,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>2024</v>
       </c>
@@ -6226,7 +6228,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>2025</v>
       </c>
@@ -6258,7 +6260,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>2026</v>
       </c>
@@ -6290,7 +6292,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>2027</v>
       </c>
@@ -6322,7 +6324,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>2028</v>
       </c>
@@ -6354,7 +6356,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>2029</v>
       </c>
@@ -6386,7 +6388,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>2030</v>
       </c>
@@ -6418,7 +6420,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>2031</v>
       </c>
@@ -6450,7 +6452,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>2032</v>
       </c>
@@ -6482,7 +6484,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>2033</v>
       </c>
@@ -6514,7 +6516,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>2034</v>
       </c>
@@ -6546,7 +6548,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>2035</v>
       </c>
@@ -6578,7 +6580,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>2036</v>
       </c>
@@ -6610,7 +6612,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>2037</v>
       </c>
@@ -6642,7 +6644,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>2038</v>
       </c>
@@ -6674,7 +6676,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>2039</v>
       </c>
@@ -6706,7 +6708,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>2040</v>
       </c>
@@ -6738,7 +6740,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>2041</v>
       </c>
@@ -6770,7 +6772,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>2042</v>
       </c>
@@ -6802,7 +6804,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>2043</v>
       </c>
@@ -6834,7 +6836,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>2044</v>
       </c>
@@ -6866,7 +6868,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>2045</v>
       </c>
@@ -6898,7 +6900,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>2046</v>
       </c>
@@ -6930,7 +6932,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>2047</v>
       </c>
@@ -6962,7 +6964,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>2048</v>
       </c>
@@ -6994,7 +6996,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>2049</v>
       </c>
@@ -7026,7 +7028,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>2050</v>
       </c>
@@ -7058,7 +7060,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>2022</v>
       </c>
@@ -7090,7 +7092,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>2023</v>
       </c>
@@ -7122,7 +7124,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>2024</v>
       </c>
@@ -7154,7 +7156,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>2025</v>
       </c>
@@ -7186,7 +7188,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>2026</v>
       </c>
@@ -7218,7 +7220,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>2027</v>
       </c>
@@ -7250,7 +7252,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>2028</v>
       </c>
@@ -7282,7 +7284,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>2029</v>
       </c>
@@ -7314,7 +7316,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>2030</v>
       </c>
@@ -7346,7 +7348,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>2031</v>
       </c>
@@ -7378,7 +7380,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>2032</v>
       </c>
@@ -7410,7 +7412,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>2033</v>
       </c>
@@ -7442,7 +7444,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>2034</v>
       </c>
@@ -7474,7 +7476,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>2035</v>
       </c>
@@ -7506,7 +7508,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>2036</v>
       </c>
@@ -7538,7 +7540,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>2037</v>
       </c>
@@ -7570,7 +7572,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>2038</v>
       </c>
@@ -7602,7 +7604,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>2039</v>
       </c>
@@ -7634,7 +7636,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>2040</v>
       </c>
@@ -7666,7 +7668,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>2041</v>
       </c>
@@ -7698,7 +7700,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>2042</v>
       </c>
@@ -7730,7 +7732,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>2043</v>
       </c>
@@ -7762,7 +7764,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>2044</v>
       </c>
@@ -7794,7 +7796,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>2045</v>
       </c>
@@ -7826,7 +7828,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>2046</v>
       </c>
@@ -7858,7 +7860,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>2047</v>
       </c>
@@ -7890,7 +7892,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>2048</v>
       </c>
@@ -7922,7 +7924,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A232" s="1">
         <v>2049</v>
       </c>
@@ -7954,7 +7956,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A233" s="1">
         <v>2050</v>
       </c>
@@ -7986,7 +7988,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>2022</v>
       </c>
@@ -8018,7 +8020,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A235" s="1">
         <v>2023</v>
       </c>
@@ -8050,7 +8052,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A236" s="1">
         <v>2024</v>
       </c>
@@ -8082,7 +8084,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A237" s="1">
         <v>2025</v>
       </c>
@@ -8114,7 +8116,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A238" s="1">
         <v>2026</v>
       </c>
@@ -8146,7 +8148,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A239" s="1">
         <v>2027</v>
       </c>
@@ -8178,7 +8180,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A240" s="1">
         <v>2028</v>
       </c>
@@ -8210,7 +8212,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A241" s="1">
         <v>2029</v>
       </c>
@@ -8242,7 +8244,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242" s="1">
         <v>2030</v>
       </c>
@@ -8274,7 +8276,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A243" s="1">
         <v>2031</v>
       </c>
@@ -8306,7 +8308,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A244" s="1">
         <v>2032</v>
       </c>
@@ -8338,7 +8340,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A245" s="1">
         <v>2033</v>
       </c>
@@ -8370,7 +8372,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A246" s="1">
         <v>2034</v>
       </c>
@@ -8402,7 +8404,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A247" s="1">
         <v>2035</v>
       </c>
@@ -8434,7 +8436,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A248" s="1">
         <v>2036</v>
       </c>
@@ -8466,7 +8468,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A249" s="1">
         <v>2037</v>
       </c>
@@ -8498,7 +8500,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A250" s="1">
         <v>2038</v>
       </c>
@@ -8530,7 +8532,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A251" s="1">
         <v>2039</v>
       </c>
@@ -8562,7 +8564,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A252" s="1">
         <v>2040</v>
       </c>
@@ -8594,7 +8596,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253" s="1">
         <v>2041</v>
       </c>
@@ -8626,7 +8628,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254" s="1">
         <v>2042</v>
       </c>
@@ -8658,7 +8660,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A255" s="1">
         <v>2043</v>
       </c>
@@ -8690,7 +8692,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A256" s="1">
         <v>2044</v>
       </c>
@@ -8722,7 +8724,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" s="1">
         <v>2045</v>
       </c>
@@ -8754,7 +8756,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" s="1">
         <v>2046</v>
       </c>
@@ -8786,7 +8788,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" s="1">
         <v>2047</v>
       </c>
@@ -8818,7 +8820,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" s="1">
         <v>2048</v>
       </c>
@@ -8850,7 +8852,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" s="1">
         <v>2049</v>
       </c>
@@ -8882,7 +8884,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" s="1">
         <v>2050</v>
       </c>
@@ -8914,7 +8916,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" s="1">
         <v>2022</v>
       </c>
@@ -8946,7 +8948,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" s="1">
         <v>2023</v>
       </c>
@@ -8978,7 +8980,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A265" s="1">
         <v>2024</v>
       </c>
@@ -9010,7 +9012,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266" s="1">
         <v>2025</v>
       </c>
@@ -9042,7 +9044,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" s="1">
         <v>2026</v>
       </c>
@@ -9074,7 +9076,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268" s="1">
         <v>2027</v>
       </c>
@@ -9106,7 +9108,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269" s="1">
         <v>2028</v>
       </c>
@@ -9138,7 +9140,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" s="1">
         <v>2029</v>
       </c>
@@ -9170,7 +9172,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" s="1">
         <v>2030</v>
       </c>
@@ -9202,7 +9204,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" s="1">
         <v>2031</v>
       </c>
@@ -9234,7 +9236,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A273" s="1">
         <v>2032</v>
       </c>
@@ -9266,7 +9268,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A274" s="1">
         <v>2033</v>
       </c>
@@ -9298,7 +9300,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" s="1">
         <v>2034</v>
       </c>
@@ -9330,7 +9332,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A276" s="1">
         <v>2035</v>
       </c>
@@ -9362,7 +9364,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A277" s="1">
         <v>2036</v>
       </c>
@@ -9394,7 +9396,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A278" s="1">
         <v>2037</v>
       </c>
@@ -9426,7 +9428,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A279" s="1">
         <v>2038</v>
       </c>
@@ -9458,7 +9460,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A280" s="1">
         <v>2039</v>
       </c>
@@ -9490,7 +9492,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A281" s="1">
         <v>2040</v>
       </c>
@@ -9522,7 +9524,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A282" s="1">
         <v>2041</v>
       </c>
@@ -9554,7 +9556,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A283" s="1">
         <v>2042</v>
       </c>
@@ -9586,7 +9588,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A284" s="1">
         <v>2043</v>
       </c>
@@ -9618,7 +9620,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A285" s="1">
         <v>2044</v>
       </c>
@@ -9650,7 +9652,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A286" s="1">
         <v>2045</v>
       </c>
@@ -9682,7 +9684,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A287" s="1">
         <v>2046</v>
       </c>
@@ -9714,7 +9716,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A288" s="1">
         <v>2047</v>
       </c>
@@ -9746,7 +9748,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A289" s="1">
         <v>2048</v>
       </c>
@@ -9778,7 +9780,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A290" s="1">
         <v>2049</v>
       </c>
@@ -9810,7 +9812,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A291" s="1">
         <v>2050</v>
       </c>
@@ -9842,7 +9844,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A292" s="1">
         <v>2022</v>
       </c>
@@ -9874,7 +9876,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A293" s="1">
         <v>2023</v>
       </c>
@@ -9906,7 +9908,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A294" s="1">
         <v>2024</v>
       </c>
@@ -9938,7 +9940,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A295" s="1">
         <v>2025</v>
       </c>
@@ -9970,7 +9972,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A296" s="1">
         <v>2026</v>
       </c>
@@ -10002,7 +10004,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A297" s="1">
         <v>2027</v>
       </c>
@@ -10034,7 +10036,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A298" s="1">
         <v>2028</v>
       </c>
@@ -10066,7 +10068,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A299" s="1">
         <v>2029</v>
       </c>
@@ -10098,7 +10100,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A300" s="1">
         <v>2030</v>
       </c>
@@ -10130,7 +10132,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A301" s="1">
         <v>2031</v>
       </c>
@@ -10162,7 +10164,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A302" s="1">
         <v>2032</v>
       </c>
@@ -10194,7 +10196,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A303" s="1">
         <v>2033</v>
       </c>
@@ -10226,7 +10228,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A304" s="1">
         <v>2034</v>
       </c>
@@ -10258,7 +10260,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="305" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A305" s="1">
         <v>2035</v>
       </c>
@@ -10290,7 +10292,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A306" s="1">
         <v>2036</v>
       </c>
@@ -10322,7 +10324,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A307" s="1">
         <v>2037</v>
       </c>
@@ -10354,7 +10356,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="308" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A308" s="1">
         <v>2038</v>
       </c>
@@ -10386,7 +10388,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="309" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A309" s="1">
         <v>2039</v>
       </c>
@@ -10418,7 +10420,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="310" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A310" s="1">
         <v>2040</v>
       </c>
@@ -10450,7 +10452,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="311" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A311" s="1">
         <v>2041</v>
       </c>
@@ -10482,7 +10484,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="312" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A312" s="1">
         <v>2042</v>
       </c>
@@ -10514,7 +10516,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="313" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A313" s="1">
         <v>2043</v>
       </c>
@@ -10546,7 +10548,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="314" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A314" s="1">
         <v>2044</v>
       </c>
@@ -10578,7 +10580,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="315" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A315" s="1">
         <v>2045</v>
       </c>
@@ -10610,7 +10612,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="316" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A316" s="1">
         <v>2046</v>
       </c>
@@ -10642,7 +10644,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="317" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A317" s="1">
         <v>2047</v>
       </c>
@@ -10674,7 +10676,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="318" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A318" s="1">
         <v>2048</v>
       </c>
@@ -10706,7 +10708,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="319" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A319" s="1">
         <v>2049</v>
       </c>
@@ -10738,7 +10740,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="320" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A320" s="1">
         <v>2050</v>
       </c>
@@ -10783,9 +10785,9 @@
       <selection activeCell="A23" sqref="A23:J81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10877,7 +10879,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -10969,7 +10971,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -11061,7 +11063,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -11153,7 +11155,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -11245,7 +11247,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -11337,7 +11339,7 @@
         <v>14.5</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -11429,7 +11431,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -11521,7 +11523,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -11613,7 +11615,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -11705,7 +11707,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -11797,7 +11799,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -11889,7 +11891,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
@@ -11981,7 +11983,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>4</v>
       </c>
@@ -12073,7 +12075,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>5</v>
       </c>
@@ -12165,7 +12167,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>6</v>
       </c>
@@ -12257,7 +12259,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
@@ -12349,7 +12351,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
@@ -12441,7 +12443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>12</v>
       </c>
@@ -12473,7 +12475,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>2022</v>
       </c>
@@ -12505,7 +12507,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>2023</v>
       </c>
@@ -12537,7 +12539,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>2024</v>
       </c>
@@ -12569,7 +12571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>2025</v>
       </c>
@@ -12601,7 +12603,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>2026</v>
       </c>
@@ -12633,7 +12635,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>2027</v>
       </c>
@@ -12665,7 +12667,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>2028</v>
       </c>
@@ -12697,7 +12699,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>2029</v>
       </c>
@@ -12729,7 +12731,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>2030</v>
       </c>
@@ -12761,7 +12763,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>2031</v>
       </c>
@@ -12793,7 +12795,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>2032</v>
       </c>
@@ -12825,7 +12827,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>2033</v>
       </c>
@@ -12857,7 +12859,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>2034</v>
       </c>
@@ -12889,7 +12891,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>2035</v>
       </c>
@@ -12921,7 +12923,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>2036</v>
       </c>
@@ -12953,7 +12955,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>2037</v>
       </c>
@@ -12985,7 +12987,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>2038</v>
       </c>
@@ -13017,7 +13019,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>2039</v>
       </c>
@@ -13049,7 +13051,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>2040</v>
       </c>
@@ -13081,7 +13083,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>2041</v>
       </c>
@@ -13113,7 +13115,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>2042</v>
       </c>
@@ -13145,7 +13147,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>2043</v>
       </c>
@@ -13177,7 +13179,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>2044</v>
       </c>
@@ -13209,7 +13211,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>2045</v>
       </c>
@@ -13241,7 +13243,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>2046</v>
       </c>
@@ -13273,7 +13275,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>2047</v>
       </c>
@@ -13305,7 +13307,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>2048</v>
       </c>
@@ -13337,7 +13339,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>2049</v>
       </c>
@@ -13369,7 +13371,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>2050</v>
       </c>
@@ -13401,7 +13403,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>2022</v>
       </c>
@@ -13433,7 +13435,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>2023</v>
       </c>
@@ -13465,7 +13467,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>2024</v>
       </c>
@@ -13497,7 +13499,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>2025</v>
       </c>
@@ -13529,7 +13531,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>2026</v>
       </c>
@@ -13561,7 +13563,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>2027</v>
       </c>
@@ -13593,7 +13595,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>2028</v>
       </c>
@@ -13625,7 +13627,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>2029</v>
       </c>
@@ -13657,7 +13659,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>2030</v>
       </c>
@@ -13689,7 +13691,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>2031</v>
       </c>
@@ -13721,7 +13723,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>2032</v>
       </c>
@@ -13753,7 +13755,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>2033</v>
       </c>
@@ -13785,7 +13787,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>2034</v>
       </c>
@@ -13817,7 +13819,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>2035</v>
       </c>
@@ -13849,7 +13851,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>2036</v>
       </c>
@@ -13881,7 +13883,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>2037</v>
       </c>
@@ -13913,7 +13915,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>2038</v>
       </c>
@@ -13945,7 +13947,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>2039</v>
       </c>
@@ -13977,7 +13979,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>2040</v>
       </c>
@@ -14009,7 +14011,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>2041</v>
       </c>
@@ -14041,7 +14043,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>2042</v>
       </c>
@@ -14073,7 +14075,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>2043</v>
       </c>
@@ -14105,7 +14107,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>2044</v>
       </c>
@@ -14137,7 +14139,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>2045</v>
       </c>
@@ -14169,7 +14171,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>2046</v>
       </c>
@@ -14201,7 +14203,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>2047</v>
       </c>
@@ -14233,7 +14235,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>2048</v>
       </c>
@@ -14265,7 +14267,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>2049</v>
       </c>
@@ -14297,7 +14299,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>2050</v>
       </c>

</xml_diff>